<commit_message>
ExcelData completed and added groups for tests
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -5,14 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KSLT018\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KSLT018\IdeaProjects\ShopLocal_Project\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CustomerLoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="CustomerRegistrationData" sheetId="2" r:id="rId2"/>
+    <sheet name="AddressData" sheetId="3" r:id="rId3"/>
+    <sheet name="CardDetailsData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,9 +26,86 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>priyapattem99@gmail.com</t>
+  </si>
+  <si>
+    <t>Krify@123</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>phNumber</t>
+  </si>
+  <si>
+    <t>City Name</t>
+  </si>
+  <si>
+    <t>State Name</t>
+  </si>
+  <si>
+    <t>Country Name</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>swathi</t>
+  </si>
+  <si>
+    <t>swathipriya@krify.com</t>
+  </si>
+  <si>
+    <t>CardHolderName</t>
+  </si>
+  <si>
+    <t>CardHolderAddress</t>
+  </si>
+  <si>
+    <t>CardHolderNumber</t>
+  </si>
+  <si>
+    <t>CardExpirymonth</t>
+  </si>
+  <si>
+    <t>cardExpiryYear</t>
+  </si>
+  <si>
+    <t>CardCvv</t>
+  </si>
+  <si>
+    <t>sarpavaram</t>
+  </si>
+  <si>
+    <t>kakinada</t>
+  </si>
+  <si>
+    <t>Andhra pradesh</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,13 +113,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -51,13 +157,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -336,12 +457,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6">
+        <v>9705688455</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2">
+        <v>533005</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="17" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6">
+        <v>411111111111111</v>
+      </c>
+      <c r="D2" s="6">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6">
+        <v>23</v>
+      </c>
+      <c r="F2" s="6">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates testdata exccel file
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerLoginData" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>username</t>
   </si>
@@ -99,13 +99,28 @@
   </si>
   <si>
     <t>Canada</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>priya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +135,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -161,7 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -175,6 +196,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -463,13 +487,13 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -496,19 +520,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>9705688455</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -520,7 +595,7 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
@@ -532,7 +607,7 @@
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -558,7 +633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -596,11 +671,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
@@ -610,7 +685,7 @@
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -630,7 +705,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>12</v>
       </c>

</xml_diff>